<commit_message>
Avances en aplicacion backend
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\Desktop\Proyectos\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE5AC3C-F98E-4B96-B68B-45BAABC98CF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F023996-7E18-4BB4-9D18-3D62CA373BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Fecha</t>
   </si>
@@ -63,6 +63,36 @@
   </si>
   <si>
     <t>Interfaces graficas con Tkinte, sqlite</t>
+  </si>
+  <si>
+    <t>Patron MVC</t>
+  </si>
+  <si>
+    <t>Patron mvc inicio de proyectoen php</t>
+  </si>
+  <si>
+    <t>Creación de primeras funciones</t>
+  </si>
+  <si>
+    <t>Enrutador para nuestra aplicación</t>
+  </si>
+  <si>
+    <t>Creación de varios controllers</t>
+  </si>
+  <si>
+    <t>Controllers</t>
+  </si>
+  <si>
+    <t>Modelos</t>
+  </si>
+  <si>
+    <t>Creación de varios modelos</t>
+  </si>
+  <si>
+    <t>Interface</t>
+  </si>
+  <si>
+    <t>Creacion de interface para crud</t>
   </si>
 </sst>
 </file>
@@ -199,17 +229,17 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -527,8 +557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,11 +569,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
@@ -560,307 +590,380 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="6">
         <v>44727</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="6">
         <v>44729</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="6">
         <v>44730</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6">
+        <v>44732</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="12" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
+      <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="6">
+        <v>44733</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
+      <c r="C15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="6">
+        <v>44734</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="6">
+        <v>44735</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="18" spans="3:5" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="C19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="6">
+        <v>44736</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
     </row>
     <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-      <c r="E34" s="7"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-      <c r="E36" s="7"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="7"/>
-      <c r="D38" s="7"/>
-      <c r="E38" s="7"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="3:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="7"/>
-      <c r="D40" s="7"/>
-      <c r="E40" s="7"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="7"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="3:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="3:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="7"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="7"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="7"/>
-      <c r="D50" s="7"/>
-      <c r="E50" s="7"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" spans="3:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-      <c r="E52" s="7"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="3:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="7"/>
-      <c r="D54" s="7"/>
-      <c r="E54" s="7"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="7"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
     </row>
     <row r="58" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="7"/>
-      <c r="D58" s="7"/>
-      <c r="E58" s="7"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -876,61 +979,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Avance en proyecto php
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\Desktop\Proyectos\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29590DEB-54DD-41DF-A142-D51733813BFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D3E113-E94E-46B0-A908-AD9D73B94A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Fecha</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Creacion de Views</t>
+  </si>
+  <si>
+    <t>Creacion de modelo de modelos expenses y categorias</t>
   </si>
 </sst>
 </file>
@@ -235,9 +238,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -246,6 +246,9 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -563,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,11 +578,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
@@ -596,343 +599,392 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>44727</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>44729</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>44730</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>44732</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>44733</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>44734</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>44735</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>44736</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>44737</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
+      <c r="C23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="6">
+        <v>46931</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
     </row>
     <row r="26" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
     </row>
     <row r="28" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
     </row>
     <row r="30" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
     </row>
     <row r="32" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="3:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="3:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="3:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" spans="3:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="3:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
     </row>
     <row r="58" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -948,61 +1000,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
creacion de modelo join
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\Desktop\Proyectos\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64D3E113-E94E-46B0-A908-AD9D73B94A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F188AA89-F9D1-41A0-92FC-1F69A63DB31F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Fecha</t>
   </si>
@@ -101,7 +101,10 @@
     <t>Creacion de Views</t>
   </si>
   <si>
-    <t>Creacion de modelo de modelos expenses y categorias</t>
+    <t>Creacion de modelo join para la consulta en BD</t>
+  </si>
+  <si>
+    <t>Creacion de modelos expenses y categorias</t>
   </si>
 </sst>
 </file>
@@ -238,6 +241,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -246,9 +252,6 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -566,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,11 +581,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
@@ -599,392 +602,355 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>44727</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>44729</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="7">
         <v>44730</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="7">
         <v>44732</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="7">
         <v>44733</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="7">
         <v>44734</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="7">
         <v>44735</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="7">
         <v>44736</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="7">
         <v>44737</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="6">
-        <v>46931</v>
-      </c>
-      <c r="E23" s="4" t="s">
+      <c r="D23" s="7">
+        <v>44739</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="7">
+        <v>44740</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-    </row>
     <row r="26" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
     </row>
     <row r="28" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
     </row>
     <row r="30" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
     </row>
     <row r="34" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="3:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" spans="3:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
     </row>
     <row r="46" spans="3:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="3:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="3:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -1000,18 +966,61 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Avance de proyecto php
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\Desktop\Proyectos\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{583C858A-8497-444F-B27D-B08667559DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A995D5-6326-438B-8915-B8B1A9EF06C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Fecha</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Creacion de controller y views de user</t>
+  </si>
+  <si>
+    <t>Controller</t>
+  </si>
+  <si>
+    <t>Creacion de controller de administrador</t>
   </si>
 </sst>
 </file>
@@ -250,9 +256,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -261,6 +264,9 @@
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -579,7 +585,7 @@
   <dimension ref="C2:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:E30"/>
+      <selection activeCell="E31" sqref="E31:E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,11 +596,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
@@ -611,367 +617,416 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="6">
         <v>44727</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
     </row>
     <row r="7" spans="3:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>44729</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>44730</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="6">
         <v>44732</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="7">
+      <c r="D13" s="6">
         <v>44733</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="7">
+      <c r="D15" s="6">
         <v>44734</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
     <row r="17" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>44735</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <v>44736</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D21" s="6">
         <v>44737</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="6">
         <v>44739</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="E23" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="7">
+      <c r="D25" s="6">
         <v>44740</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
     </row>
     <row r="27" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="7">
+      <c r="D27" s="6">
         <v>44741</v>
       </c>
-      <c r="E27" s="5" t="s">
+      <c r="E27" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="7">
+      <c r="D29" s="6">
         <v>44742</v>
       </c>
-      <c r="E29" s="5" t="s">
+      <c r="E29" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
+      <c r="C31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="6">
+        <v>44713</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="32" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
     </row>
     <row r="34" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
     </row>
     <row r="36" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
     </row>
     <row r="38" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
     </row>
     <row r="40" spans="3:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
     </row>
     <row r="42" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
     </row>
     <row r="44" spans="3:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
     </row>
     <row r="46" spans="3:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
     </row>
     <row r="48" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
     </row>
     <row r="50" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
     </row>
     <row r="52" spans="3:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
-      <c r="E52" s="6"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
     </row>
     <row r="54" spans="3:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
     </row>
     <row r="56" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
     </row>
     <row r="58" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -987,61 +1042,18 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finalizacion de de proyecto php
</commit_message>
<xml_diff>
--- a/Bitacora.xlsx
+++ b/Bitacora.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\Desktop\Proyectos\bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A995D5-6326-438B-8915-B8B1A9EF06C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A31F004F-E1C2-46EC-8CE6-A389ACF9683D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{5F60A4A5-F201-4BBE-B609-D8E3E8F91B78}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>Fecha</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Creacion de controller de administrador</t>
+  </si>
+  <si>
+    <t>Finalizacion</t>
+  </si>
+  <si>
+    <t>Fin de proyecto</t>
   </si>
 </sst>
 </file>
@@ -245,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -256,6 +262,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -265,8 +274,8 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -584,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0452DAB7-0726-4DA6-A9FD-B8609C601486}">
   <dimension ref="C2:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31:E32"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33:E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,11 +605,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:5" ht="36" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="3:5" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
@@ -617,416 +626,379 @@
       </c>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="7">
         <v>44727</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="3:5" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
     </row>
     <row r="7" spans="3:5" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="7">
         <v>44729</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="3:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="7">
         <v>44730</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="3:5" ht="35.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+      <c r="C11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="7">
         <v>44732</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="E11" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
     </row>
     <row r="13" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="7">
         <v>44733</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="E13" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="14" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="7">
         <v>44734</v>
       </c>
-      <c r="E15" s="4" t="s">
+      <c r="E15" s="5" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+      <c r="C17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="7">
         <v>44735</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="E17" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="3:5" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="4" t="s">
+      <c r="C19" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="6">
+      <c r="D19" s="7">
         <v>44736</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="E19" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="3:5" ht="38.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
     </row>
     <row r="21" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="7">
         <v>44737</v>
       </c>
-      <c r="E21" s="4" t="s">
+      <c r="E21" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="22" spans="3:5" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="6">
+      <c r="D23" s="7">
         <v>44739</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="24" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
+      <c r="C25" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="6">
+      <c r="D25" s="7">
         <v>44740</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E25" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="26" spans="3:5" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
     </row>
     <row r="27" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="4" t="s">
+      <c r="C27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="7">
         <v>44741</v>
       </c>
-      <c r="E27" s="4" t="s">
+      <c r="E27" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="28" spans="3:5" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C29" s="4" t="s">
+      <c r="C29" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="7">
         <v>44742</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="30" spans="3:5" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" s="4" t="s">
+      <c r="C31" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="7">
         <v>44713</v>
       </c>
-      <c r="E31" s="4" t="s">
+      <c r="E31" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="32" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
+      <c r="C33" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D33" s="8">
+        <v>44746</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="34" spans="3:5" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
     </row>
     <row r="36" spans="3:5" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
     </row>
     <row r="38" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" spans="3:5" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C41" s="4"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
     </row>
     <row r="42" spans="3:5" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
     </row>
     <row r="44" spans="3:5" ht="41.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
     </row>
     <row r="46" spans="3:5" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
     </row>
     <row r="48" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="3:5" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
     </row>
     <row r="52" spans="3:5" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
     </row>
     <row r="54" spans="3:5" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="3:5" ht="42.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="3:5" ht="45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="C17:C18"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="D21:D22"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="E23:E24"/>
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="D25:D26"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="C27:C28"/>
-    <mergeCell ref="D27:D28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="C31:C32"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="E31:E32"/>
-    <mergeCell ref="C33:C34"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="E35:E36"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
     <mergeCell ref="C49:C50"/>
     <mergeCell ref="D49:D50"/>
     <mergeCell ref="E49:E50"/>
@@ -1042,18 +1014,61 @@
     <mergeCell ref="C47:C48"/>
     <mergeCell ref="D47:D48"/>
     <mergeCell ref="E47:E48"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="E35:E36"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="C31:C32"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="E31:E32"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>